<commit_message>
Updated BOM and Sensor Matrix
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rct47/volcanic-ash-uav/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\My Uni Work\3rd Pro\ENMT401\volcanic-ash-uav\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="19200" windowHeight="7836" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Overall Total</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Shipping(nzd)</t>
   </si>
   <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/9689</t>
-  </si>
-  <si>
     <t>Sharp Optical Dust Sensor</t>
   </si>
   <si>
@@ -84,14 +78,40 @@
   </si>
   <si>
     <t>Shpping (nzd)</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/Free-Shipping-PM2-5-GP2Y1010AU0F-SENSOR-AIR-QUALITY-DUST-GP2Y10-Compact-Optical-Dust-Sensor-Smoke-Particle/32314774144.html?spm=2114.01010208.3.47.T9wGdx&amp;ws_ab_test=searchweb201556_0,searchweb201602_3_10017_10005_10006_10034_10021_507_10022_10020_10018_10019,searchweb201603_9&amp;btsid=0f96a037-dd7a-4cb8-8149-8bec116ef816</t>
+  </si>
+  <si>
+    <t>Plantower PMS5003 Laser Dust Sensor</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/PLANTOWER-PM2-5-SENSOR-laser-dust-sensor-G5-PMS5003-High-precision-laser-dust-concentration-sensor-digital/32618735056.html?spm=2114.01010208.3.10.wbvLWe&amp;ws_ab_test=searchweb201556_0,searchweb201602_3_10017_10005_10006_10034_10021_507_10022_10020_10018_10019,searchweb201603_9&amp;btsid=8b09eea3-1bb7-4347-b788-b4bbf9f0939b</t>
+  </si>
+  <si>
+    <t>Nova SDS011 Laser Dust Sensor</t>
+  </si>
+  <si>
+    <t>AliExpress (HS Electronics)</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/nova-PM-sensor-SDS011-High-precision-laser-pm2-5-air-quality-detection-sensor-module-Super-dust/32617788139.html?spm=2114.01010208.3.20.gbKqjW&amp;ws_ab_test=searchweb201556_0,searchweb201602_3_10017_10005_10006_10034_10021_507_10022_10020_10018_10019,searchweb201603_9&amp;btsid=0144ffea-7eee-4de0-8be5-b055fc86186a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,6 +151,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -398,37 +422,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:N11"/>
+  <dimension ref="C4:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="50.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" customWidth="1"/>
+    <col min="7" max="7" width="51.5" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" customWidth="1"/>
+    <col min="13" max="13" width="13.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4">
         <f>SUM(E5,L5)</f>
-        <v>443</v>
-      </c>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
+        <v>513.1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5">
-        <f>SUM(D9:D11,F9:F11)</f>
-        <v>443</v>
+        <f>SUM(D9:D13,F9:F13)</f>
+        <v>513.1</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
@@ -438,7 +463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -446,7 +471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -454,20 +479,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J8" t="s">
@@ -480,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -500,7 +525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -511,27 +536,62 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>15</v>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>36.4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM (Added Shinyei sensor)
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
-  <si>
-    <t>Overall Total</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Order 1</t>
   </si>
@@ -47,9 +44,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Order Total</t>
-  </si>
-  <si>
     <t>Order 2</t>
   </si>
   <si>
@@ -68,12 +62,6 @@
     <t>PixHawk GPS</t>
   </si>
   <si>
-    <t>Shipping(nzd)</t>
-  </si>
-  <si>
-    <t>Sharp Optical Dust Sensor</t>
-  </si>
-  <si>
     <t>https://store.3dr.com/products/3dr-gps-ublox-with-compass</t>
   </si>
   <si>
@@ -96,6 +84,39 @@
   </si>
   <si>
     <t>http://www.aliexpress.com/item/nova-PM-sensor-SDS011-High-precision-laser-pm2-5-air-quality-detection-sensor-module-Super-dust/32617788139.html?spm=2114.01010208.3.20.gbKqjW&amp;ws_ab_test=searchweb201556_0,searchweb201602_3_10017_10005_10006_10034_10021_507_10022_10020_10018_10019,searchweb201603_9&amp;btsid=0144ffea-7eee-4de0-8be5-b055fc86186a</t>
+  </si>
+  <si>
+    <t>Shinyei PPD42NS</t>
+  </si>
+  <si>
+    <t>Sharp GP2Y1010AU0F Optical Dust Sensor</t>
+  </si>
+  <si>
+    <t>Cost (USD)</t>
+  </si>
+  <si>
+    <t>Overall Total (approx, NZD)</t>
+  </si>
+  <si>
+    <t>Exchange rate used (approx NZD per USD)</t>
+  </si>
+  <si>
+    <t>Cost (approx NZD)</t>
+  </si>
+  <si>
+    <t>Order 1 Total (approx, NZD)</t>
+  </si>
+  <si>
+    <t>Order 2 Total (approx, NZD)</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/Japan-imported-spot-SHINYEI-PM2-5-dust-sensor-PPD42-PPD42NJ-PPD42NS-PPD4NS-with-cable/32616905622.html?spm=2114.40010508.4.2.VozAhD</t>
+  </si>
+  <si>
+    <t>Shipping (USD)</t>
+  </si>
+  <si>
+    <t>Shipping (approx NZD)</t>
   </si>
 </sst>
 </file>
@@ -422,172 +443,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M13"/>
+  <dimension ref="B3:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="13.296875" customWidth="1"/>
-    <col min="6" max="6" width="51.5" customWidth="1"/>
-    <col min="9" max="9" width="13.796875" customWidth="1"/>
-    <col min="12" max="12" width="13.296875" customWidth="1"/>
+    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="3" max="3" width="11.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" customWidth="1"/>
+    <col min="7" max="7" width="19.8984375" customWidth="1"/>
+    <col min="8" max="8" width="51.5" customWidth="1"/>
+    <col min="11" max="11" width="22.8984375" customWidth="1"/>
+    <col min="14" max="14" width="13.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <f>SUM(D5,K5)</f>
-        <v>513.1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <f>SUM(C20,L20)</f>
+        <v>515.18500000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
-        <f>SUM(C9:C13,E9:E13)</f>
-        <v>513.1</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="K8" t="s">
         <v>6</v>
       </c>
-      <c r="K5">
-        <f>SUM(J9:J11,L9:L11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C11">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <f>$C11*$C$5</f>
+        <v>290</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>$F11*$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
         <v>8</v>
       </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <f>$C12*$C$5</f>
+        <v>130.5</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>290</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>$F12*$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>130</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13">
-        <v>36.4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
+        <v>6.8</v>
+      </c>
+      <c r="D13">
+        <f>$C13*$C$5</f>
+        <v>9.86</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>$F13*$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <f>$C14*$C$5</f>
+        <v>47.85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>$F14*$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>25.5</v>
+      </c>
+      <c r="D15">
+        <f>$C15*$C$5</f>
+        <v>36.975000000000001</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>$F15*$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>10.5</v>
+      </c>
+      <c r="D16">
+        <f>$C16*$C$5</f>
+        <v>15.225</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>$F16*$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <f>SUM(D11:D15,G11:G15)</f>
+        <v>515.18500000000006</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20">
+        <f>SUM(L11:L13,N11:N13)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>